<commit_message>
Initial Scripts w Succesful Python Invocation
</commit_message>
<xml_diff>
--- a/ML_RPA_UiPathCode_Process_Legacy/Input/Test_Question_File.3_15.xlsx
+++ b/ML_RPA_UiPathCode_Process_Legacy/Input/Test_Question_File.3_15.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <x:si>
     <x:t>Code</x:t>
   </x:si>
@@ -74,51 +74,69 @@
     <x:t>Yes;No;Refused;Don't Know;Missing</x:t>
   </x:si>
   <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KIQ005</x:t>
+  </x:si>
+  <x:si>
+    <x:t>How Often Do You Have Urinary Leakage per week?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Never;Less than once a month;A few times a month;A few times a week; Ever day and/or night; Refused;Don't Know;Missing</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Ever day and/or night</x:t>
+  </x:si>
+  <x:si>
+    <x:t>None</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AUQ054</x:t>
+  </x:si>
+  <x:si>
+    <x:t>General Condition of Hearing?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Excellent;Good;A little trouble;Moderate hearing trouble;A lot of trouble;Deaf;Refused;Don't Know;Missing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Excellent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCQ560</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Have You Ever Had GallBladder Surgery?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCQ371D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Are you watching your weight?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HUQ071</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Were you a Patient in Hospital Overnight? Not including emergency Room</x:t>
+  </x:si>
+  <x:si>
     <x:t>Don't Know</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
   </x:si>
   <x:si>
-    <x:t>KIQ005</x:t>
-  </x:si>
-  <x:si>
-    <x:t>How Often Do You Have Urinary Leakage per week?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Never;Less than once a month;A few times a month;A few times a week; Ever day and/or night; Refused;Don't Know;Missing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AUQ054</x:t>
-  </x:si>
-  <x:si>
-    <x:t>General Condition of Hearing?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Excellent;Good;A little trouble;Moderate hearing trouble;A lot of trouble;Deaf;Refused;Don't Know;Missing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>99</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCQ560</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Have You Ever Had GallBladder Surgery?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCQ371D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Are you watching your weight?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HUQ071</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Were you a Patient in Hospital Overnight? Not including emergency Room</x:t>
-  </x:si>
-  <x:si>
     <x:t>OHQ033</x:t>
   </x:si>
   <x:si>
@@ -128,6 +146,9 @@
     <x:t>Went in on own for check-up, examination, or cleaning;Was called in by dentist for check-up, examination, or cleaning;Something was wrong, bothering, or hurting; Went for treatment of a condition that dentist previously discovered;Other;Refused;Don't Know;Missing</x:t>
   </x:si>
   <x:si>
+    <x:t>Went in on own for check-up, examination, or cleaning</x:t>
+  </x:si>
+  <x:si>
     <x:t>MCQ092</x:t>
   </x:si>
   <x:si>
@@ -149,6 +170,9 @@
     <x:t>Not at all;Several Days;More than half the days;Nearly every day;Refused;Don't Know;Missing</x:t>
   </x:si>
   <x:si>
+    <x:t>More than half the days</x:t>
+  </x:si>
+  <x:si>
     <x:t>PUQ110</x:t>
   </x:si>
   <x:si>
@@ -164,7 +188,10 @@
     <x:t>None;1;2 to 3;4 to 5;6 to 7;8 to 9;10 to 12;13 to 15;16 or more;Refused;Don't Know;Missing</x:t>
   </x:si>
   <x:si>
-    <x:t>None</x:t>
+    <x:t>10 to 12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -615,92 +642,92 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A4" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A5" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A6" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A7" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A8" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>9</x:v>
@@ -708,10 +735,10 @@
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A9" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
         <x:v>7</x:v>
@@ -725,44 +752,44 @@
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A10" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A11" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A12" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
         <x:v>7</x:v>
@@ -776,19 +803,19 @@
     </x:row>
     <x:row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <x:c r="A13" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>